<commit_message>
First cut of cycle processing
</commit_message>
<xml_diff>
--- a/source_data/berber_1_v2.xlsx
+++ b/source_data/berber_1_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3D57FB-8FF1-494C-8DB5-1EC79211C3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B8F309-4A1B-EC40-91E6-7899A951D716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13220" yWindow="500" windowWidth="41380" windowHeight="23400" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -144,15 +144,6 @@
   </si>
   <si>
     <t>Day 46</t>
-  </si>
-  <si>
-    <t>A: Day 1</t>
-  </si>
-  <si>
-    <t>A: Day 16</t>
-  </si>
-  <si>
-    <t>P4: +30 Days</t>
   </si>
   <si>
     <t>P1: +14 Days</t>
@@ -587,7 +578,7 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,7 +628,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F2" s="9">
         <v>1</v>
@@ -655,13 +646,13 @@
         <v>6</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -669,10 +660,10 @@
       <c r="B3" s="10"/>
       <c r="C3" s="7"/>
       <c r="D3" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>9</v>
@@ -690,13 +681,13 @@
         <v>35</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -707,7 +698,7 @@
         <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>30</v>
@@ -728,10 +719,10 @@
         <v>30</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -742,31 +733,31 @@
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -780,34 +771,34 @@
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="O6" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -818,7 +809,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
@@ -848,7 +839,7 @@
         <v>13</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -859,10 +850,10 @@
         <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>15</v>
@@ -903,21 +894,21 @@
         <v>28</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>25</v>
@@ -925,16 +916,16 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>25</v>
@@ -945,7 +936,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>20</v>
@@ -954,7 +945,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>25</v>
@@ -986,35 +977,35 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>